<commit_message>
Small updates to the Results file
</commit_message>
<xml_diff>
--- a/RawData/Results.xlsx
+++ b/RawData/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rhvt/Dev/SUNA/gym-uds-api/RawData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{DCC0DE59-E552-5645-9F8E-6F9059603FEC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{9296B3A0-D5B1-EC44-B87A-CDB495E3E31B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{DE3548C4-FDD8-E942-B840-C87F182DD8E1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" activeTab="4" xr2:uid="{DE3548C4-FDD8-E942-B840-C87F182DD8E1}"/>
   </bookViews>
   <sheets>
     <sheet name="MountainCar-V0" sheetId="1" r:id="rId1"/>
@@ -1338,7 +1338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E60D2105-5C86-474C-AEF4-0BBD7F940641}">
   <dimension ref="A1:U115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J115" sqref="J115:L115"/>
     </sheetView>
   </sheetViews>
@@ -105960,7 +105960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E2F3F23-73AA-5A44-8B1A-63CD119A59DA}">
   <dimension ref="A1:V65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>

</xml_diff>